<commit_message>
copysheet and style changes
</commit_message>
<xml_diff>
--- a/website_app/copysheet.xlsx
+++ b/website_app/copysheet.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Bills" sheetId="1" r:id="rId1"/>
     <sheet name="Legislators" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -2107,8 +2102,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2432,12 +2427,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -4732,21 +4727,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -6209,10 +6199,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>